<commit_message>
Africa Cup of Nations and Copa Centroamericana 2017
Africa Cup of Nations and Copa Centroamericana 2017
</commit_message>
<xml_diff>
--- a/Scripts/copacentroamericana/copacentroamericana.xlsx
+++ b/Scripts/copacentroamericana/copacentroamericana.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -9785,7 +9785,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -9801,566 +9801,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
       <c r="G1" t="str">
-        <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A1 &amp; ", '" &amp; B1 &amp; "', " &amp; C1 &amp; ", " &amp; D1 &amp;  ");"</f>
-        <v>insert into game (matchid, matchdate, game_type, country) values (matchid, 'matchdate', game_type, country);</v>
+        <f>"insert into group_stage (id, tournament, group_code, squad) values (" &amp; A1 &amp; ", " &amp; B1 &amp; ", '" &amp; C1 &amp; "', " &amp; D1 &amp;  ");"</f>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (id, tournament, 'group_code', squad);</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'2014'!A22+1</f>
-        <v>170</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f>"2017-01-13"</f>
-        <v>2017-01-13</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
+        <f>'2014'!A8+1</f>
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>2017</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>507</v>
+        <v>505</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G16" si="0">"insert into game (matchid, matchdate, game_type, country) values (" &amp; A2 &amp; ", '" &amp; B2 &amp; "', " &amp; C2 &amp; ", " &amp; D2 &amp;  ");"</f>
-        <v>insert into game (matchid, matchdate, game_type, country) values (170, '2017-01-13', 2, 507);</v>
+        <f t="shared" ref="G2:G7" si="0">"insert into group_stage (id, tournament, group_code, squad) values (" &amp; A2 &amp; ", " &amp; B2 &amp; ", '" &amp; C2 &amp; "', " &amp; D2 &amp;  ");"</f>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (68, 2017, 'A', 505);</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
-        <v>171</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f>"2017-01-13"</f>
-        <v>2017-01-13</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <f t="shared" ref="A3:A7" si="1">A2+1</f>
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B7" si="2">B2</f>
+        <v>2017</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>insert into game (matchid, matchdate, game_type, country) values (171, '2017-01-13', 2, 507);</v>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (69, 2017, 'A', 503);</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A16" si="1">A3+1</f>
-        <v>172</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>"2017-01-13"</f>
-        <v>2017-01-13</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>insert into game (matchid, matchdate, game_type, country) values (172, '2017-01-13', 2, 507);</v>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (70, 2017, 'A', 504);</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>173</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f>"2017-01-15"</f>
-        <v>2017-01-15</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into game (matchid, matchdate, game_type, country) values (173, '2017-01-15', 2, 507);</v>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (71, 2017, 'A', 501);</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>174</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f>"2017-01-15"</f>
-        <v>2017-01-15</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>insert into game (matchid, matchdate, game_type, country) values (174, '2017-01-15', 2, 507);</v>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (72, 2017, 'A', 506);</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="B7" s="2" t="str">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>507</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into group_stage (id, tournament, group_code, squad) values (73, 2017, 'A', 507);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="str">
+        <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A9 &amp; ", '" &amp; B9 &amp; "', " &amp; C9 &amp; ", " &amp; D9 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (matchid, 'matchdate', game_type, country);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>'2014'!A22+1</f>
+        <v>170</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>"2017-01-13"</f>
+        <v>2017-01-13</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>507</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10:G24" si="3">"insert into game (matchid, matchdate, game_type, country) values (" &amp; A10 &amp; ", '" &amp; B10 &amp; "', " &amp; C10 &amp; ", " &amp; D10 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (170, '2017-01-13', 2, 507);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10+1</f>
+        <v>171</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>"2017-01-13"</f>
+        <v>2017-01-13</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>507</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (171, '2017-01-13', 2, 507);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ref="A12:A24" si="4">A11+1</f>
+        <v>172</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>"2017-01-13"</f>
+        <v>2017-01-13</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>507</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (172, '2017-01-13', 2, 507);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="4"/>
+        <v>173</v>
+      </c>
+      <c r="B13" s="2" t="str">
         <f>"2017-01-15"</f>
         <v>2017-01-15</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>507</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
+      <c r="G13" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (173, '2017-01-15', 2, 507);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>"2017-01-15"</f>
+        <v>2017-01-15</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>507</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (174, '2017-01-15', 2, 507);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>"2017-01-15"</f>
+        <v>2017-01-15</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>507</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (175, '2017-01-15', 2, 507);</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="1"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="4"/>
         <v>176</v>
       </c>
-      <c r="B8" s="2" t="str">
+      <c r="B16" s="2" t="str">
         <f>"2017-01-17"</f>
         <v>2017-01-17</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
         <v>507</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
+      <c r="G16" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (176, '2017-01-17', 2, 507);</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="1"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="4"/>
         <v>177</v>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B17" s="2" t="str">
         <f>"2017-01-17"</f>
         <v>2017-01-17</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
         <v>507</v>
       </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
+      <c r="G17" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (177, '2017-01-17', 2, 507);</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="1"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="4"/>
         <v>178</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B18" s="2" t="str">
         <f>"2017-01-17"</f>
         <v>2017-01-17</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
         <v>507</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
+      <c r="G18" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (178, '2017-01-17', 2, 507);</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="1"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="4"/>
         <v>179</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B19" s="2" t="str">
         <f>"2017-01-20"</f>
         <v>2017-01-20</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
         <v>507</v>
       </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (179, '2017-01-20', 2, 507);</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="1"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
-      <c r="B12" s="2" t="str">
+      <c r="B20" s="2" t="str">
         <f>"2017-01-20"</f>
         <v>2017-01-20</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
         <v>507</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (180, '2017-01-20', 2, 507);</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="1"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="4"/>
         <v>181</v>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B21" s="2" t="str">
         <f>"2017-01-20"</f>
         <v>2017-01-20</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
         <v>507</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (181, '2017-01-20', 2, 507);</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B22" s="2" t="str">
         <f>"2017-01-22"</f>
         <v>2017-01-22</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
         <v>507</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
+      <c r="G22" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (182, '2017-01-22', 2, 507);</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="1"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="4"/>
         <v>183</v>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B23" s="2" t="str">
         <f>"2017-01-22"</f>
         <v>2017-01-22</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
         <v>507</v>
       </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
+      <c r="G23" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (183, '2017-01-22', 2, 507);</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="1"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="4"/>
         <v>184</v>
       </c>
-      <c r="B16" s="2" t="str">
+      <c r="B24" s="2" t="str">
         <f>"2017-01-22"</f>
         <v>2017-01-22</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
         <v>507</v>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
+      <c r="G24" t="str">
+        <f t="shared" si="3"/>
         <v>insert into game (matchid, matchdate, game_type, country) values (184, '2017-01-22', 2, 507);</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G18" t="str">
-        <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A18 &amp; ", " &amp; B18 &amp; ", " &amp; C18 &amp; ", " &amp; D18 &amp; ", " &amp; E18 &amp; ", " &amp; F18 &amp; ");"</f>
+      <c r="G26" t="str">
+        <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A26 &amp; ", " &amp; B26 &amp; ", " &amp; C26 &amp; ", " &amp; D26 &amp; ", " &amp; E26 &amp; ", " &amp; F26 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (id, matchid, squad, goals, points, time_type);</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <f>'2014'!A72 + 1</f>
         <v>689</v>
       </c>
-      <c r="B19" s="3">
-        <f>A2</f>
+      <c r="B27" s="3">
+        <f>A10</f>
         <v>170</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C27" s="3">
         <v>504</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="3">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="str">
-        <f t="shared" ref="G19:G78" si="2">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A19 &amp; ", " &amp; B19 &amp; ", " &amp; C19 &amp; ", " &amp; D19 &amp; ", " &amp; E19 &amp; ", " &amp; F19 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (689, 170, 504, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <f>A19+1</f>
-        <v>690</v>
-      </c>
-      <c r="B20" s="3">
-        <f>B19</f>
-        <v>170</v>
-      </c>
-      <c r="C20" s="3">
-        <v>504</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (690, 170, 504, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <f t="shared" ref="A21:A78" si="3">A20+1</f>
-        <v>691</v>
-      </c>
-      <c r="B21" s="3">
-        <f>B19</f>
-        <v>170</v>
-      </c>
-      <c r="C21" s="3">
-        <v>505</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="3">
-        <v>2</v>
-      </c>
-      <c r="G21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (691, 170, 505, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <f t="shared" si="3"/>
-        <v>692</v>
-      </c>
-      <c r="B22" s="3">
-        <f>B19</f>
-        <v>170</v>
-      </c>
-      <c r="C22" s="3">
-        <v>505</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (692, 170, 505, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <f>A22+1</f>
-        <v>693</v>
-      </c>
-      <c r="B23" s="4">
-        <f>B19+1</f>
-        <v>171</v>
-      </c>
-      <c r="C23" s="4">
-        <v>506</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="4">
-        <v>2</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (693, 171, 506, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <f t="shared" si="3"/>
-        <v>694</v>
-      </c>
-      <c r="B24" s="4">
-        <f>B23</f>
-        <v>171</v>
-      </c>
-      <c r="C24" s="4">
-        <v>506</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (694, 171, 506, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <f t="shared" si="3"/>
-        <v>695</v>
-      </c>
-      <c r="B25" s="4">
-        <f>B23</f>
-        <v>171</v>
-      </c>
-      <c r="C25" s="4">
-        <v>503</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="4">
-        <v>2</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (695, 171, 503, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <f t="shared" si="3"/>
-        <v>696</v>
-      </c>
-      <c r="B26" s="4">
-        <f>B23</f>
-        <v>171</v>
-      </c>
-      <c r="C26" s="4">
-        <v>503</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (696, 171, 503, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <f t="shared" si="3"/>
-        <v>697</v>
-      </c>
-      <c r="B27" s="3">
-        <f>B23+1</f>
-        <v>172</v>
-      </c>
-      <c r="C27" s="3">
-        <v>507</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>9</v>
@@ -10372,21 +10304,21 @@
         <v>2</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (697, 172, 507, null, null, 2);</v>
+        <f t="shared" ref="G27:G86" si="5">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A27 &amp; ", " &amp; B27 &amp; ", " &amp; C27 &amp; ", " &amp; D27 &amp; ", " &amp; E27 &amp; ", " &amp; F27 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (689, 170, 504, null, null, 2);</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <f t="shared" si="3"/>
-        <v>698</v>
+        <f>A27+1</f>
+        <v>690</v>
       </c>
       <c r="B28" s="3">
         <f>B27</f>
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C28" s="3">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
@@ -10398,21 +10330,21 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (698, 172, 507, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (690, 170, 504, null, null, 1);</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <f t="shared" si="3"/>
-        <v>699</v>
+        <f t="shared" ref="A29:A86" si="6">A28+1</f>
+        <v>691</v>
       </c>
       <c r="B29" s="3">
         <f>B27</f>
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C29" s="3">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>9</v>
@@ -10424,21 +10356,21 @@
         <v>2</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (699, 172, 501, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (691, 170, 505, null, null, 2);</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <f t="shared" si="3"/>
-        <v>700</v>
+        <f t="shared" si="6"/>
+        <v>692</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" ref="B30" si="4">B27</f>
-        <v>172</v>
+        <f>B27</f>
+        <v>170</v>
       </c>
       <c r="C30" s="3">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>9</v>
@@ -10450,21 +10382,21 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (700, 172, 501, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (692, 170, 505, null, null, 1);</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f t="shared" si="3"/>
-        <v>701</v>
+        <f>A30+1</f>
+        <v>693</v>
       </c>
       <c r="B31" s="4">
         <f>B27+1</f>
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C31" s="4">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>9</v>
@@ -10475,22 +10407,22 @@
       <c r="F31" s="4">
         <v>2</v>
       </c>
-      <c r="G31" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (701, 173, 501, null, null, 2);</v>
+      <c r="G31" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (693, 171, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f t="shared" si="3"/>
-        <v>702</v>
+        <f t="shared" si="6"/>
+        <v>694</v>
       </c>
       <c r="B32" s="4">
         <f>B31</f>
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C32" s="4">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>9</v>
@@ -10501,22 +10433,22 @@
       <c r="F32" s="4">
         <v>1</v>
       </c>
-      <c r="G32" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (702, 173, 501, null, null, 1);</v>
+      <c r="G32" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (694, 171, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <f t="shared" si="3"/>
-        <v>703</v>
+        <f t="shared" si="6"/>
+        <v>695</v>
       </c>
       <c r="B33" s="4">
         <f>B31</f>
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C33" s="4">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
@@ -10527,22 +10459,22 @@
       <c r="F33" s="4">
         <v>2</v>
       </c>
-      <c r="G33" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (703, 173, 506, null, null, 2);</v>
+      <c r="G33" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (695, 171, 503, null, null, 2);</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <f t="shared" si="3"/>
-        <v>704</v>
+        <f t="shared" si="6"/>
+        <v>696</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" ref="B34" si="5">B31</f>
-        <v>173</v>
+        <f>B31</f>
+        <v>171</v>
       </c>
       <c r="C34" s="4">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>9</v>
@@ -10553,22 +10485,22 @@
       <c r="F34" s="4">
         <v>1</v>
       </c>
-      <c r="G34" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (704, 173, 506, null, null, 1);</v>
+      <c r="G34" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (696, 171, 503, null, null, 1);</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <f t="shared" si="3"/>
-        <v>705</v>
+        <f t="shared" si="6"/>
+        <v>697</v>
       </c>
       <c r="B35" s="3">
         <f>B31+1</f>
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C35" s="3">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>9</v>
@@ -10580,21 +10512,21 @@
         <v>2</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (705, 174, 503, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (697, 172, 507, null, null, 2);</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <f t="shared" si="3"/>
-        <v>706</v>
+        <f t="shared" si="6"/>
+        <v>698</v>
       </c>
       <c r="B36" s="3">
         <f>B35</f>
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C36" s="3">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>9</v>
@@ -10606,21 +10538,21 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (706, 174, 503, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (698, 172, 507, null, null, 1);</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <f t="shared" si="3"/>
-        <v>707</v>
+        <f t="shared" si="6"/>
+        <v>699</v>
       </c>
       <c r="B37" s="3">
         <f>B35</f>
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C37" s="3">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>9</v>
@@ -10632,21 +10564,21 @@
         <v>2</v>
       </c>
       <c r="G37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (707, 174, 504, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (699, 172, 501, null, null, 2);</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <f t="shared" si="3"/>
-        <v>708</v>
+        <f t="shared" si="6"/>
+        <v>700</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" ref="B38" si="6">B35</f>
-        <v>174</v>
+        <f t="shared" ref="B38" si="7">B35</f>
+        <v>172</v>
       </c>
       <c r="C38" s="3">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>9</v>
@@ -10658,21 +10590,21 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (708, 174, 504, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (700, 172, 501, null, null, 1);</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <f t="shared" si="3"/>
-        <v>709</v>
+        <f t="shared" si="6"/>
+        <v>701</v>
       </c>
       <c r="B39" s="4">
         <f>B35+1</f>
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C39" s="4">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -10684,21 +10616,21 @@
         <v>2</v>
       </c>
       <c r="G39" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (709, 175, 507, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (701, 173, 501, null, null, 2);</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <f t="shared" si="3"/>
-        <v>710</v>
+        <f t="shared" si="6"/>
+        <v>702</v>
       </c>
       <c r="B40" s="4">
         <f>B39</f>
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C40" s="4">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -10710,21 +10642,21 @@
         <v>1</v>
       </c>
       <c r="G40" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (710, 175, 507, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (702, 173, 501, null, null, 1);</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <f t="shared" si="3"/>
-        <v>711</v>
+        <f t="shared" si="6"/>
+        <v>703</v>
       </c>
       <c r="B41" s="4">
         <f>B39</f>
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C41" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
@@ -10736,21 +10668,21 @@
         <v>2</v>
       </c>
       <c r="G41" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (711, 175, 505, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (703, 173, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <f t="shared" si="3"/>
-        <v>712</v>
+        <f t="shared" si="6"/>
+        <v>704</v>
       </c>
       <c r="B42" s="4">
-        <f t="shared" ref="B42" si="7">B39</f>
-        <v>175</v>
+        <f t="shared" ref="B42" si="8">B39</f>
+        <v>173</v>
       </c>
       <c r="C42" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
@@ -10762,18 +10694,18 @@
         <v>1</v>
       </c>
       <c r="G42" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (712, 175, 505, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (704, 173, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <f t="shared" si="3"/>
-        <v>713</v>
+        <f t="shared" si="6"/>
+        <v>705</v>
       </c>
       <c r="B43" s="3">
         <f>B39+1</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" s="3">
         <v>503</v>
@@ -10788,18 +10720,18 @@
         <v>2</v>
       </c>
       <c r="G43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (713, 176, 503, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (705, 174, 503, null, null, 2);</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <f t="shared" si="3"/>
-        <v>714</v>
+        <f t="shared" si="6"/>
+        <v>706</v>
       </c>
       <c r="B44" s="3">
         <f>B43</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C44" s="3">
         <v>503</v>
@@ -10814,21 +10746,21 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (714, 176, 503, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (706, 174, 503, null, null, 1);</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <f t="shared" si="3"/>
-        <v>715</v>
+        <f t="shared" si="6"/>
+        <v>707</v>
       </c>
       <c r="B45" s="3">
         <f>B43</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C45" s="3">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>9</v>
@@ -10840,21 +10772,21 @@
         <v>2</v>
       </c>
       <c r="G45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (715, 176, 501, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (707, 174, 504, null, null, 2);</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <f t="shared" si="3"/>
-        <v>716</v>
+        <f t="shared" si="6"/>
+        <v>708</v>
       </c>
       <c r="B46" s="3">
-        <f t="shared" ref="B46" si="8">B43</f>
-        <v>176</v>
+        <f t="shared" ref="B46" si="9">B43</f>
+        <v>174</v>
       </c>
       <c r="C46" s="3">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>9</v>
@@ -10866,21 +10798,21 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (716, 176, 501, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (708, 174, 504, null, null, 1);</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <f t="shared" si="3"/>
-        <v>717</v>
+        <f t="shared" si="6"/>
+        <v>709</v>
       </c>
       <c r="B47" s="4">
         <f>B43+1</f>
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C47" s="4">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>9</v>
@@ -10892,21 +10824,21 @@
         <v>2</v>
       </c>
       <c r="G47" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (717, 177, 506, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (709, 175, 507, null, null, 2);</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <f t="shared" si="3"/>
-        <v>718</v>
+        <f t="shared" si="6"/>
+        <v>710</v>
       </c>
       <c r="B48" s="4">
         <f>B47</f>
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C48" s="4">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>9</v>
@@ -10918,18 +10850,18 @@
         <v>1</v>
       </c>
       <c r="G48" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (718, 177, 506, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (710, 175, 507, null, null, 1);</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <f t="shared" si="3"/>
-        <v>719</v>
+        <f t="shared" si="6"/>
+        <v>711</v>
       </c>
       <c r="B49" s="4">
         <f>B47</f>
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C49" s="4">
         <v>505</v>
@@ -10944,18 +10876,18 @@
         <v>2</v>
       </c>
       <c r="G49" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (719, 177, 505, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (711, 175, 505, null, null, 2);</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <f t="shared" si="3"/>
-        <v>720</v>
+        <f t="shared" si="6"/>
+        <v>712</v>
       </c>
       <c r="B50" s="4">
-        <f t="shared" ref="B50" si="9">B47</f>
-        <v>177</v>
+        <f t="shared" ref="B50" si="10">B47</f>
+        <v>175</v>
       </c>
       <c r="C50" s="4">
         <v>505</v>
@@ -10970,21 +10902,21 @@
         <v>1</v>
       </c>
       <c r="G50" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (720, 177, 505, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (712, 175, 505, null, null, 1);</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <f t="shared" si="3"/>
-        <v>721</v>
+        <f t="shared" si="6"/>
+        <v>713</v>
       </c>
       <c r="B51" s="3">
         <f>B47+1</f>
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C51" s="3">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>9</v>
@@ -10996,21 +10928,21 @@
         <v>2</v>
       </c>
       <c r="G51" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (721, 178, 507, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (713, 176, 503, null, null, 2);</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <f t="shared" si="3"/>
-        <v>722</v>
+        <f t="shared" si="6"/>
+        <v>714</v>
       </c>
       <c r="B52" s="3">
         <f>B51</f>
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C52" s="3">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>9</v>
@@ -11022,21 +10954,21 @@
         <v>1</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (722, 178, 507, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (714, 176, 503, null, null, 1);</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <f t="shared" si="3"/>
-        <v>723</v>
+        <f t="shared" si="6"/>
+        <v>715</v>
       </c>
       <c r="B53" s="3">
         <f>B51</f>
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C53" s="3">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>9</v>
@@ -11048,21 +10980,21 @@
         <v>2</v>
       </c>
       <c r="G53" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (723, 178, 504, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (715, 176, 501, null, null, 2);</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <f t="shared" si="3"/>
-        <v>724</v>
+        <f t="shared" si="6"/>
+        <v>716</v>
       </c>
       <c r="B54" s="3">
-        <f t="shared" ref="B54" si="10">B51</f>
-        <v>178</v>
+        <f t="shared" ref="B54" si="11">B51</f>
+        <v>176</v>
       </c>
       <c r="C54" s="3">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>9</v>
@@ -11074,21 +11006,21 @@
         <v>1</v>
       </c>
       <c r="G54" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (724, 178, 504, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (716, 176, 501, null, null, 1);</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <f t="shared" si="3"/>
-        <v>725</v>
+        <f t="shared" si="6"/>
+        <v>717</v>
       </c>
       <c r="B55" s="4">
         <f>B51+1</f>
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C55" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
@@ -11100,21 +11032,21 @@
         <v>2</v>
       </c>
       <c r="G55" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (725, 179, 505, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (717, 177, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <f t="shared" si="3"/>
-        <v>726</v>
+        <f t="shared" si="6"/>
+        <v>718</v>
       </c>
       <c r="B56" s="4">
         <f>B55</f>
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C56" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
@@ -11126,21 +11058,21 @@
         <v>1</v>
       </c>
       <c r="G56" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (726, 179, 505, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (718, 177, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <f t="shared" si="3"/>
-        <v>727</v>
+        <f t="shared" si="6"/>
+        <v>719</v>
       </c>
       <c r="B57" s="4">
         <f>B55</f>
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C57" s="4">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
@@ -11152,21 +11084,21 @@
         <v>2</v>
       </c>
       <c r="G57" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (727, 179, 501, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (719, 177, 505, null, null, 2);</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <f t="shared" si="3"/>
-        <v>728</v>
+        <f t="shared" si="6"/>
+        <v>720</v>
       </c>
       <c r="B58" s="4">
-        <f t="shared" ref="B58" si="11">B55</f>
-        <v>179</v>
+        <f t="shared" ref="B58" si="12">B55</f>
+        <v>177</v>
       </c>
       <c r="C58" s="4">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -11178,21 +11110,21 @@
         <v>1</v>
       </c>
       <c r="G58" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (728, 179, 501, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (720, 177, 505, null, null, 1);</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <f t="shared" si="3"/>
-        <v>729</v>
+        <f t="shared" si="6"/>
+        <v>721</v>
       </c>
       <c r="B59" s="3">
         <f>B55+1</f>
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C59" s="3">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>9</v>
@@ -11204,21 +11136,21 @@
         <v>2</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (729, 180, 504, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (721, 178, 507, null, null, 2);</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <f t="shared" si="3"/>
-        <v>730</v>
+        <f t="shared" si="6"/>
+        <v>722</v>
       </c>
       <c r="B60" s="3">
         <f>B59</f>
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C60" s="3">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>9</v>
@@ -11230,21 +11162,21 @@
         <v>1</v>
       </c>
       <c r="G60" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (730, 180, 504, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (722, 178, 507, null, null, 1);</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <f t="shared" si="3"/>
-        <v>731</v>
+        <f t="shared" si="6"/>
+        <v>723</v>
       </c>
       <c r="B61" s="3">
         <f>B59</f>
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C61" s="3">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>9</v>
@@ -11256,21 +11188,21 @@
         <v>2</v>
       </c>
       <c r="G61" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (731, 180, 506, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (723, 178, 504, null, null, 2);</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <f t="shared" si="3"/>
-        <v>732</v>
+        <f t="shared" si="6"/>
+        <v>724</v>
       </c>
       <c r="B62" s="3">
-        <f t="shared" ref="B62" si="12">B59</f>
-        <v>180</v>
+        <f t="shared" ref="B62" si="13">B59</f>
+        <v>178</v>
       </c>
       <c r="C62" s="3">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>9</v>
@@ -11282,21 +11214,21 @@
         <v>1</v>
       </c>
       <c r="G62" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (732, 180, 506, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (724, 178, 504, null, null, 1);</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <f t="shared" si="3"/>
-        <v>733</v>
+        <f t="shared" si="6"/>
+        <v>725</v>
       </c>
       <c r="B63" s="4">
         <f>B59+1</f>
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C63" s="4">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
@@ -11308,21 +11240,21 @@
         <v>2</v>
       </c>
       <c r="G63" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (733, 181, 507, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (725, 179, 505, null, null, 2);</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <f t="shared" si="3"/>
-        <v>734</v>
+        <f t="shared" si="6"/>
+        <v>726</v>
       </c>
       <c r="B64" s="4">
         <f>B63</f>
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C64" s="4">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
@@ -11334,21 +11266,21 @@
         <v>1</v>
       </c>
       <c r="G64" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (734, 181, 507, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (726, 179, 505, null, null, 1);</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <f t="shared" si="3"/>
-        <v>735</v>
+        <f t="shared" si="6"/>
+        <v>727</v>
       </c>
       <c r="B65" s="4">
         <f>B63</f>
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C65" s="4">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>9</v>
@@ -11360,21 +11292,21 @@
         <v>2</v>
       </c>
       <c r="G65" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (735, 181, 503, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (727, 179, 501, null, null, 2);</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <f t="shared" si="3"/>
-        <v>736</v>
+        <f t="shared" si="6"/>
+        <v>728</v>
       </c>
       <c r="B66" s="4">
-        <f t="shared" ref="B66" si="13">B63</f>
-        <v>181</v>
+        <f t="shared" ref="B66" si="14">B63</f>
+        <v>179</v>
       </c>
       <c r="C66" s="4">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>9</v>
@@ -11386,21 +11318,21 @@
         <v>1</v>
       </c>
       <c r="G66" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (736, 181, 503, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (728, 179, 501, null, null, 1);</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <f t="shared" si="3"/>
-        <v>737</v>
+        <f t="shared" si="6"/>
+        <v>729</v>
       </c>
       <c r="B67" s="3">
         <f>B63+1</f>
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C67" s="3">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>9</v>
@@ -11412,21 +11344,21 @@
         <v>2</v>
       </c>
       <c r="G67" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (737, 182, 501, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (729, 180, 504, null, null, 2);</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <f t="shared" si="3"/>
-        <v>738</v>
+        <f t="shared" si="6"/>
+        <v>730</v>
       </c>
       <c r="B68" s="3">
         <f>B67</f>
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C68" s="3">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>9</v>
@@ -11438,21 +11370,21 @@
         <v>1</v>
       </c>
       <c r="G68" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (738, 182, 501, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (730, 180, 504, null, null, 1);</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <f t="shared" si="3"/>
-        <v>739</v>
+        <f t="shared" si="6"/>
+        <v>731</v>
       </c>
       <c r="B69" s="3">
         <f>B67</f>
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C69" s="3">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>9</v>
@@ -11464,21 +11396,21 @@
         <v>2</v>
       </c>
       <c r="G69" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (739, 182, 504, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (731, 180, 506, null, null, 2);</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <f t="shared" si="3"/>
-        <v>740</v>
+        <f t="shared" si="6"/>
+        <v>732</v>
       </c>
       <c r="B70" s="3">
-        <f t="shared" ref="B70" si="14">B67</f>
-        <v>182</v>
+        <f t="shared" ref="B70" si="15">B67</f>
+        <v>180</v>
       </c>
       <c r="C70" s="3">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>9</v>
@@ -11490,21 +11422,21 @@
         <v>1</v>
       </c>
       <c r="G70" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (740, 182, 504, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (732, 180, 506, null, null, 1);</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <f t="shared" si="3"/>
-        <v>741</v>
+        <f t="shared" si="6"/>
+        <v>733</v>
       </c>
       <c r="B71" s="4">
         <f>B67+1</f>
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C71" s="4">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>9</v>
@@ -11516,21 +11448,21 @@
         <v>2</v>
       </c>
       <c r="G71" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (741, 183, 503, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (733, 181, 507, null, null, 2);</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <f t="shared" si="3"/>
-        <v>742</v>
+        <f t="shared" si="6"/>
+        <v>734</v>
       </c>
       <c r="B72" s="4">
         <f>B71</f>
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C72" s="4">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>9</v>
@@ -11542,21 +11474,21 @@
         <v>1</v>
       </c>
       <c r="G72" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (742, 183, 503, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (734, 181, 507, null, null, 1);</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <f t="shared" si="3"/>
-        <v>743</v>
+        <f t="shared" si="6"/>
+        <v>735</v>
       </c>
       <c r="B73" s="4">
         <f>B71</f>
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C73" s="4">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>9</v>
@@ -11568,21 +11500,21 @@
         <v>2</v>
       </c>
       <c r="G73" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (743, 183, 505, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (735, 181, 503, null, null, 2);</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <f t="shared" si="3"/>
-        <v>744</v>
+        <f t="shared" si="6"/>
+        <v>736</v>
       </c>
       <c r="B74" s="4">
-        <f t="shared" ref="B74" si="15">B71</f>
-        <v>183</v>
+        <f t="shared" ref="B74" si="16">B71</f>
+        <v>181</v>
       </c>
       <c r="C74" s="4">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>9</v>
@@ -11594,21 +11526,21 @@
         <v>1</v>
       </c>
       <c r="G74" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (744, 183, 505, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (736, 181, 503, null, null, 1);</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <f t="shared" si="3"/>
-        <v>745</v>
+        <f t="shared" si="6"/>
+        <v>737</v>
       </c>
       <c r="B75" s="3">
         <f>B71+1</f>
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C75" s="3">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>9</v>
@@ -11620,21 +11552,21 @@
         <v>2</v>
       </c>
       <c r="G75" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (745, 184, 507, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (737, 182, 501, null, null, 2);</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <f t="shared" si="3"/>
-        <v>746</v>
+        <f t="shared" si="6"/>
+        <v>738</v>
       </c>
       <c r="B76" s="3">
         <f>B75</f>
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C76" s="3">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>9</v>
@@ -11646,21 +11578,21 @@
         <v>1</v>
       </c>
       <c r="G76" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (746, 184, 507, null, null, 1);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (738, 182, 501, null, null, 1);</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <f t="shared" si="3"/>
-        <v>747</v>
+        <f t="shared" si="6"/>
+        <v>739</v>
       </c>
       <c r="B77" s="3">
         <f>B75</f>
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C77" s="3">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>9</v>
@@ -11672,21 +11604,21 @@
         <v>2</v>
       </c>
       <c r="G77" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (747, 184, 506, null, null, 2);</v>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (739, 182, 504, null, null, 2);</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <f t="shared" si="3"/>
-        <v>748</v>
+        <f t="shared" si="6"/>
+        <v>740</v>
       </c>
       <c r="B78" s="3">
-        <f t="shared" ref="B78" si="16">B75</f>
-        <v>184</v>
+        <f t="shared" ref="B78" si="17">B75</f>
+        <v>182</v>
       </c>
       <c r="C78" s="3">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>9</v>
@@ -11698,7 +11630,215 @@
         <v>1</v>
       </c>
       <c r="G78" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (740, 182, 504, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <f t="shared" si="6"/>
+        <v>741</v>
+      </c>
+      <c r="B79" s="4">
+        <f>B75+1</f>
+        <v>183</v>
+      </c>
+      <c r="C79" s="4">
+        <v>503</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="4">
+        <v>2</v>
+      </c>
+      <c r="G79" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (741, 183, 503, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <f t="shared" si="6"/>
+        <v>742</v>
+      </c>
+      <c r="B80" s="4">
+        <f>B79</f>
+        <v>183</v>
+      </c>
+      <c r="C80" s="4">
+        <v>503</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="4">
+        <v>1</v>
+      </c>
+      <c r="G80" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (742, 183, 503, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <f t="shared" si="6"/>
+        <v>743</v>
+      </c>
+      <c r="B81" s="4">
+        <f>B79</f>
+        <v>183</v>
+      </c>
+      <c r="C81" s="4">
+        <v>505</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="4">
+        <v>2</v>
+      </c>
+      <c r="G81" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (743, 183, 505, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <f t="shared" si="6"/>
+        <v>744</v>
+      </c>
+      <c r="B82" s="4">
+        <f t="shared" ref="B82" si="18">B79</f>
+        <v>183</v>
+      </c>
+      <c r="C82" s="4">
+        <v>505</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="4">
+        <v>1</v>
+      </c>
+      <c r="G82" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (744, 183, 505, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <f t="shared" si="6"/>
+        <v>745</v>
+      </c>
+      <c r="B83" s="3">
+        <f>B79+1</f>
+        <v>184</v>
+      </c>
+      <c r="C83" s="3">
+        <v>507</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="3">
+        <v>2</v>
+      </c>
+      <c r="G83" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (745, 184, 507, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <f t="shared" si="6"/>
+        <v>746</v>
+      </c>
+      <c r="B84" s="3">
+        <f>B83</f>
+        <v>184</v>
+      </c>
+      <c r="C84" s="3">
+        <v>507</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1</v>
+      </c>
+      <c r="G84" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (746, 184, 507, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <f t="shared" si="6"/>
+        <v>747</v>
+      </c>
+      <c r="B85" s="3">
+        <f>B83</f>
+        <v>184</v>
+      </c>
+      <c r="C85" s="3">
+        <v>506</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="3">
+        <v>2</v>
+      </c>
+      <c r="G85" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (747, 184, 506, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <f t="shared" si="6"/>
+        <v>748</v>
+      </c>
+      <c r="B86" s="3">
+        <f t="shared" ref="B86" si="19">B83</f>
+        <v>184</v>
+      </c>
+      <c r="C86" s="3">
+        <v>506</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (748, 184, 506, null, null, 1);</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Copa Centroamericana more issues fixed
Copa Centroamericana more issues fixed
</commit_message>
<xml_diff>
--- a/Scripts/copacentroamericana/copacentroamericana.xlsx
+++ b/Scripts/copacentroamericana/copacentroamericana.xlsx
@@ -435,9 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23491,14 +23489,14 @@
         <v>2</v>
       </c>
       <c r="E54" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F54" s="4">
         <v>2</v>
       </c>
       <c r="G54" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (383, 96, 506, 2, 0, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (383, 96, 506, 2, 3, 2);</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -23543,14 +23541,14 @@
         <v>1</v>
       </c>
       <c r="E56" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F56" s="4">
         <v>2</v>
       </c>
       <c r="G56" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (385, 96, 503, 1, 3, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (385, 96, 503, 1, 0, 2);</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Copa Centroamericana First Date Results
Copa Centroamericana First Date Results
</commit_message>
<xml_diff>
--- a/Scripts/copacentroamericana/copacentroamericana.xlsx
+++ b/Scripts/copacentroamericana/copacentroamericana.xlsx
@@ -10501,14 +10501,14 @@
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3">
         <v>2</v>
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (697, 172, 507, 0, 0, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (697, 172, 507, 0, 1, 2);</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -10553,14 +10553,14 @@
         <v>0</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3">
         <v>2</v>
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (699, 172, 501, 0, 0, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (699, 172, 501, 0, 1, 2);</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>